<commit_message>
change: reran test case and pasted terminal output
</commit_message>
<xml_diff>
--- a/unit_tests.xlsx
+++ b/unit_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanb\DLSU\YEAR_2\TERM_3\LBYARCH\MP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1E1C138A-84F8-4822-AD22-10A987C938B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFE9ABF-5430-45C2-9003-C65DE3D6CF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{A40A7516-F7C5-43FD-9010-216B4B96B373}"/>
   </bookViews>
@@ -17,7 +17,20 @@
     <sheet name="N=2^24" sheetId="4" r:id="rId2"/>
     <sheet name="N=2^29" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -912,7 +925,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -946,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="C2">
         <v>3.0000000000000001E-3</v>
@@ -956,11 +969,11 @@
       </c>
       <c r="F2">
         <f>AVERAGE(B2:B31)</f>
-        <v>4.0666666666666689E-3</v>
+        <v>4.1666666666666692E-3</v>
       </c>
       <c r="G2">
         <f>AVERAGE(C2:C31)</f>
-        <v>2.700000000000001E-3</v>
+        <v>2.6000000000000012E-3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -968,10 +981,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C3">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -1000,11 +1013,11 @@
       </c>
       <c r="F4">
         <f>_xlfn.STDEV.S(B2:B31)</f>
-        <v>5.8329228098567495E-4</v>
+        <v>6.9893186157624608E-4</v>
       </c>
       <c r="G4">
         <f>_xlfn.STDEV.S(C2:C31)</f>
-        <v>7.0221324985780646E-4</v>
+        <v>6.2145546626586547E-4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1015,7 +1028,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C5">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -1037,7 +1050,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C7">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1045,10 +1058,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C8">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -1056,7 +1069,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>6.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="C9">
         <v>2E-3</v>
@@ -1070,7 +1083,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C10">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -1092,7 +1105,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C12">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1103,7 +1116,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C13">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1114,7 +1127,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C14">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1125,7 +1138,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C15">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1136,7 +1149,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C16">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1147,7 +1160,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C17">
-        <v>5.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1169,7 +1182,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C19">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1177,7 +1190,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C20">
         <v>3.0000000000000001E-3</v>
@@ -1188,10 +1201,10 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>6.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C21">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1199,7 +1212,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>4.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C22">
         <v>2E-3</v>
@@ -1235,7 +1248,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C25">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1243,10 +1256,10 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>4.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C26">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1268,7 +1281,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C28">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1279,7 +1292,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C29">
-        <v>3.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1287,10 +1300,10 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>4.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="C30">
-        <v>2E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -1314,7 +1327,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -1715,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB1529D-AE71-4FD8-AD80-F5561379678F}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -1750,21 +1763,21 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5.7240000000000002</v>
+        <v>5.3369999999999997</v>
       </c>
       <c r="C2">
-        <v>7.1289999999999996</v>
+        <v>10.098000000000001</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2">
         <f>AVERAGE(B2:B31)</f>
-        <v>4.2242333333333342</v>
+        <v>5.382766666666666</v>
       </c>
       <c r="G2">
         <f>AVERAGE(C2:C31)</f>
-        <v>4.9122666666666666</v>
+        <v>5.1398999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1772,21 +1785,21 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4.4359999999999999</v>
+        <v>4.0739999999999998</v>
       </c>
       <c r="C3">
-        <v>4.7789999999999999</v>
+        <v>4.5359999999999996</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3">
         <f>MEDIAN(B2:B31)</f>
-        <v>3.9409999999999998</v>
+        <v>5.54</v>
       </c>
       <c r="G3">
         <f>MEDIAN(C2:C31)</f>
-        <v>3.8940000000000001</v>
+        <v>4.9930000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1794,21 +1807,21 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3.9</v>
+        <v>4.1070000000000002</v>
       </c>
       <c r="C4">
-        <v>5.9989999999999997</v>
+        <v>3.694</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4">
         <f>_xlfn.STDEV.S(B2:B31)</f>
-        <v>0.57623071788119595</v>
+        <v>1.4049303500550345</v>
       </c>
       <c r="G4">
         <f>_xlfn.STDEV.S(C2:C31)</f>
-        <v>2.3781005160353952</v>
+        <v>1.6060767008351464</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1816,10 +1829,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4.53</v>
+        <v>3.9359999999999999</v>
       </c>
       <c r="C5">
-        <v>4.8239999999999998</v>
+        <v>3.851</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -1827,10 +1840,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5.2930000000000001</v>
+        <v>3.9430000000000001</v>
       </c>
       <c r="C6">
-        <v>6.91</v>
+        <v>3.851</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -1838,10 +1851,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4.3140000000000001</v>
+        <v>3.9249999999999998</v>
       </c>
       <c r="C7">
-        <v>4.0149999999999997</v>
+        <v>3.6589999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1849,10 +1862,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4.3490000000000002</v>
+        <v>3.84</v>
       </c>
       <c r="C8">
-        <v>4.6050000000000004</v>
+        <v>4.1310000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -1860,10 +1873,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4.3929999999999998</v>
+        <v>3.887</v>
       </c>
       <c r="C9">
-        <v>4.5190000000000001</v>
+        <v>3.6819999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -1871,10 +1884,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>5.7510000000000003</v>
+        <v>3.9740000000000002</v>
       </c>
       <c r="C10">
-        <v>14.411</v>
+        <v>3.5579999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -1882,10 +1895,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5.319</v>
+        <v>4.0250000000000004</v>
       </c>
       <c r="C11">
-        <v>7.6059999999999999</v>
+        <v>3.4950000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1893,10 +1906,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4.5449999999999999</v>
+        <v>3.8969999999999998</v>
       </c>
       <c r="C12">
-        <v>3.6859999999999999</v>
+        <v>3.9390000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1904,10 +1917,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>3.944</v>
+        <v>3.758</v>
       </c>
       <c r="C13">
-        <v>3.355</v>
+        <v>4.4080000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1915,10 +1928,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>3.8639999999999999</v>
+        <v>4.0739999999999998</v>
       </c>
       <c r="C14">
-        <v>3.363</v>
+        <v>3.7730000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1926,10 +1939,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>3.9380000000000002</v>
+        <v>4.1710000000000003</v>
       </c>
       <c r="C15">
-        <v>3.3559999999999999</v>
+        <v>3.944</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1937,10 +1950,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>3.8420000000000001</v>
+        <v>6.8760000000000003</v>
       </c>
       <c r="C16">
-        <v>3.286</v>
+        <v>5.7030000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1948,10 +1961,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>4.2859999999999996</v>
+        <v>7.258</v>
       </c>
       <c r="C17">
-        <v>3.2679999999999998</v>
+        <v>6.117</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1959,10 +1972,10 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>3.8519999999999999</v>
+        <v>6.4829999999999997</v>
       </c>
       <c r="C18">
-        <v>3.2469999999999999</v>
+        <v>5.8259999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1970,10 +1983,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>3.9910000000000001</v>
+        <v>6.9509999999999996</v>
       </c>
       <c r="C19">
-        <v>3.37</v>
+        <v>6.0350000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1981,10 +1994,10 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>3.8879999999999999</v>
+        <v>6.1849999999999996</v>
       </c>
       <c r="C20">
-        <v>3.258</v>
+        <v>7.47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1992,10 +2005,10 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>3.8170000000000002</v>
+        <v>6.8810000000000002</v>
       </c>
       <c r="C21">
-        <v>3.359</v>
+        <v>5.524</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -2003,10 +2016,10 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>3.8050000000000002</v>
+        <v>6.6479999999999997</v>
       </c>
       <c r="C22">
-        <v>3.3050000000000002</v>
+        <v>6.4749999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -2014,10 +2027,10 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>3.831</v>
+        <v>7.1749999999999998</v>
       </c>
       <c r="C23">
-        <v>3.2909999999999999</v>
+        <v>5.2160000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2025,10 +2038,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>3.8370000000000002</v>
+        <v>6.8369999999999997</v>
       </c>
       <c r="C24">
-        <v>6.3140000000000001</v>
+        <v>5.5529999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -2036,10 +2049,10 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>3.7869999999999999</v>
+        <v>7.42</v>
       </c>
       <c r="C25">
-        <v>3.234</v>
+        <v>5.8380000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -2047,10 +2060,10 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>4.0469999999999997</v>
+        <v>6.2309999999999999</v>
       </c>
       <c r="C26">
-        <v>8.41</v>
+        <v>5.6260000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -2058,10 +2071,10 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>3.9340000000000002</v>
+        <v>5.9960000000000004</v>
       </c>
       <c r="C27">
-        <v>4.593</v>
+        <v>5.4139999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -2069,10 +2082,10 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>4.1849999999999996</v>
+        <v>7.1050000000000004</v>
       </c>
       <c r="C28">
-        <v>3.7730000000000001</v>
+        <v>8.7940000000000005</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -2080,10 +2093,10 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>3.8159999999999998</v>
+        <v>6.7069999999999999</v>
       </c>
       <c r="C29">
-        <v>3.5590000000000002</v>
+        <v>5.9669999999999996</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -2091,10 +2104,10 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>3.7320000000000002</v>
+        <v>4.0389999999999997</v>
       </c>
       <c r="C30">
-        <v>5.3230000000000004</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -2102,10 +2115,10 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>3.7770000000000001</v>
+        <v>5.7430000000000003</v>
       </c>
       <c r="C31">
-        <v>7.2210000000000001</v>
+        <v>4.7699999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>